<commit_message>
ore di lavoro aggiornate
</commit_message>
<xml_diff>
--- a/log/Ore_di_lavoro.xlsx
+++ b/log/Ore_di_lavoro.xlsx
@@ -1,18 +1,39 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10410"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jacopovecchi/PDS/2022t4/log/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7616DA96-3F44-7843-ACF5-D883818DA721}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Foglio1" sheetId="1" r:id="rId4"/>
-    <sheet state="visible" name="JANATH" sheetId="2" r:id="rId5"/>
+    <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
+    <sheet name="JANATH" sheetId="2" r:id="rId2"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="58">
   <si>
     <t>Ore trascorse sul progetto</t>
   </si>
@@ -181,52 +202,60 @@
   </si>
   <si>
     <t xml:space="preserve"> Studio individuale + Stesura delle bozze per le user stories </t>
+  </si>
+  <si>
+    <t xml:space="preserve">coding , testing </t>
+  </si>
+  <si>
+    <t>taiga, documentazione</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <numFmts count="3">
-    <numFmt numFmtId="164" formatCode="dd/mm/yy"/>
-    <numFmt numFmtId="165" formatCode="dd/mm/yyyy"/>
-    <numFmt numFmtId="166" formatCode="dd/mm"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="dd/mm/yyyy"/>
+    <numFmt numFmtId="165" formatCode="dd/mm"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="12.0"/>
+      <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
     <font>
-      <sz val="12.0"/>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
     </font>
     <font>
       <b/>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color rgb="FFF7981D"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
@@ -236,7 +265,7 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -252,78 +281,65 @@
     </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+  <cellXfs count="20">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="right" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="right" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="right" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="165" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="3" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="166" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0"/>
-    </xf>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normale" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -513,34 +529,39 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:H104"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="G88" sqref="G88"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col customWidth="1" min="2" max="2" width="13.38"/>
-    <col customWidth="1" min="3" max="3" width="25.13"/>
-    <col customWidth="1" min="4" max="4" width="26.0"/>
-    <col customWidth="1" min="5" max="5" width="22.63"/>
-    <col customWidth="1" min="6" max="6" width="24.88"/>
-    <col customWidth="1" min="7" max="7" width="25.0"/>
-    <col customWidth="1" min="8" max="8" width="23.88"/>
+    <col min="2" max="2" width="13.33203125" customWidth="1"/>
+    <col min="3" max="3" width="25.1640625" customWidth="1"/>
+    <col min="4" max="4" width="26" customWidth="1"/>
+    <col min="5" max="5" width="22.6640625" customWidth="1"/>
+    <col min="6" max="6" width="24.83203125" customWidth="1"/>
+    <col min="7" max="7" width="25" customWidth="1"/>
+    <col min="8" max="8" width="23.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1">
-        <v>12.0</v>
-      </c>
-    </row>
-    <row r="2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="2"/>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
@@ -550,10 +571,11 @@
       <c r="G2" s="2"/>
       <c r="H2" s="2"/>
     </row>
-    <row r="3">
-      <c r="A3" s="3" t="s">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" s="18" t="s">
         <v>0</v>
       </c>
+      <c r="B3" s="19"/>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
@@ -561,7 +583,7 @@
       <c r="G3" s="2"/>
       <c r="H3" s="2"/>
     </row>
-    <row r="4">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="2"/>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
@@ -571,7 +593,7 @@
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
     </row>
-    <row r="5">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="2"/>
       <c r="B5" s="2"/>
       <c r="C5" s="3" t="s">
@@ -593,7 +615,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>7</v>
       </c>
@@ -605,7 +627,7 @@
       <c r="G6" s="2"/>
       <c r="H6" s="2"/>
     </row>
-    <row r="7">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" s="2"/>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
@@ -615,9 +637,9 @@
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
     </row>
-    <row r="8">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" s="6">
-        <v>44655.0</v>
+        <v>44655</v>
       </c>
       <c r="B8" s="2"/>
       <c r="C8" s="3"/>
@@ -627,9 +649,9 @@
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
     </row>
-    <row r="9">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="6">
-        <v>44656.0</v>
+        <v>44656</v>
       </c>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
@@ -637,13 +659,13 @@
       <c r="E9" s="2"/>
       <c r="F9" s="2"/>
       <c r="G9" s="3">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="H9" s="2"/>
     </row>
-    <row r="10">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" s="6">
-        <v>44657.0</v>
+        <v>44657</v>
       </c>
       <c r="B10" s="2"/>
       <c r="C10" s="3"/>
@@ -651,37 +673,37 @@
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
       <c r="G10" s="3">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="H10" s="2"/>
     </row>
-    <row r="11">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" s="6">
-        <v>44658.0</v>
+        <v>44658</v>
       </c>
       <c r="B11" s="2"/>
       <c r="C11" s="3">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="D11" s="5">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="E11" s="3">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="F11" s="3">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="G11" s="3">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="H11" s="3">
-        <v>4.0</v>
-      </c>
-    </row>
-    <row r="12">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" s="6">
-        <v>44659.0</v>
+        <v>44659</v>
       </c>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
@@ -691,9 +713,9 @@
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
     </row>
-    <row r="13">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" s="6">
-        <v>44660.0</v>
+        <v>44660</v>
       </c>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
@@ -703,9 +725,9 @@
       <c r="G13" s="2"/>
       <c r="H13" s="2"/>
     </row>
-    <row r="14">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" s="6">
-        <v>44661.0</v>
+        <v>44661</v>
       </c>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
@@ -715,97 +737,97 @@
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
     </row>
-    <row r="15">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" s="6">
-        <v>44662.0</v>
+        <v>44662</v>
       </c>
       <c r="B15" s="2"/>
       <c r="C15" s="3">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="D15" s="5">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="E15" s="3">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="F15" s="3">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="G15" s="2"/>
       <c r="H15" s="2"/>
     </row>
-    <row r="16">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" s="6">
-        <v>44663.0</v>
+        <v>44663</v>
       </c>
       <c r="B16" s="2"/>
       <c r="C16" s="3">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="D16" s="5">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="E16" s="3">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="F16" s="2"/>
       <c r="G16" s="3">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="H16" s="2"/>
     </row>
-    <row r="17">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" s="6">
-        <v>44664.0</v>
+        <v>44664</v>
       </c>
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
       <c r="D17" s="5">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="E17" s="3">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="F17" s="2"/>
       <c r="G17" s="3">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="H17" s="2"/>
     </row>
-    <row r="18">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" s="6">
-        <v>44665.0</v>
+        <v>44665</v>
       </c>
       <c r="B18" s="2"/>
       <c r="C18" s="3">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="D18" s="5">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="E18" s="3">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="F18" s="3">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="G18" s="3">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="H18" s="3">
-        <v>2.0</v>
-      </c>
-    </row>
-    <row r="19">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" s="6">
-        <v>44666.0</v>
+        <v>44666</v>
       </c>
       <c r="B19" s="2"/>
       <c r="C19" s="3"/>
       <c r="D19" s="4"/>
       <c r="E19" s="3">
-        <v>6.0</v>
+        <v>6</v>
       </c>
       <c r="F19" s="3">
         <v>1.5</v>
@@ -813,9 +835,9 @@
       <c r="G19" s="2"/>
       <c r="H19" s="2"/>
     </row>
-    <row r="20">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" s="6">
-        <v>44667.0</v>
+        <v>44667</v>
       </c>
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
@@ -825,37 +847,37 @@
       <c r="G20" s="2"/>
       <c r="H20" s="2"/>
     </row>
-    <row r="21">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" s="2"/>
       <c r="B21" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C21" s="7">
-        <f t="shared" ref="C21:H21" si="1">SUM(C8:C20)</f>
+        <f t="shared" ref="C21:H21" si="0">SUM(C8:C20)</f>
         <v>14</v>
       </c>
       <c r="D21" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>13</v>
       </c>
       <c r="E21" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>20</v>
       </c>
       <c r="F21" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>12.5</v>
       </c>
       <c r="G21" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>22</v>
       </c>
       <c r="H21" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
     </row>
-    <row r="22">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" s="2"/>
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
@@ -865,7 +887,7 @@
       <c r="G22" s="2"/>
       <c r="H22" s="2"/>
     </row>
-    <row r="23">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
         <v>9</v>
       </c>
@@ -877,9 +899,9 @@
       <c r="G23" s="2"/>
       <c r="H23" s="2"/>
     </row>
-    <row r="24">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" s="9">
-        <v>44668.0</v>
+        <v>44668</v>
       </c>
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
@@ -889,7 +911,7 @@
       <c r="G24" s="2"/>
       <c r="H24" s="2"/>
     </row>
-    <row r="25">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
       <c r="D25" s="4"/>
@@ -898,9 +920,9 @@
       <c r="G25" s="2"/>
       <c r="H25" s="2"/>
     </row>
-    <row r="26">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26" s="9">
-        <v>44669.0</v>
+        <v>44669</v>
       </c>
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
@@ -909,103 +931,103 @@
       <c r="F26" s="2"/>
       <c r="H26" s="2"/>
     </row>
-    <row r="27">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
       <c r="D27" s="4"/>
       <c r="F27" s="3"/>
       <c r="H27" s="3"/>
     </row>
-    <row r="28">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B28" s="2"/>
       <c r="D28" s="10"/>
     </row>
-    <row r="29">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29" s="9">
-        <v>44670.0</v>
+        <v>44670</v>
       </c>
       <c r="D29" s="10"/>
       <c r="G29" s="3">
-        <v>4.0</v>
-      </c>
-    </row>
-    <row r="30">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D30" s="10"/>
     </row>
-    <row r="31">
+    <row r="31" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D31" s="10"/>
     </row>
-    <row r="32">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32" s="9">
-        <v>44671.0</v>
+        <v>44671</v>
       </c>
       <c r="D32" s="10"/>
       <c r="E32" s="3">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="G32" s="3">
-        <v>4.0</v>
-      </c>
-    </row>
-    <row r="33">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D33" s="10"/>
     </row>
-    <row r="34">
+    <row r="34" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D34" s="10"/>
     </row>
-    <row r="35">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A35" s="9">
-        <v>44672.0</v>
+        <v>44672</v>
       </c>
       <c r="C35" s="3">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="D35" s="5">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="E35" s="3">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="F35" s="3">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="G35" s="3">
-        <v>8.0</v>
+        <v>8</v>
       </c>
       <c r="H35" s="3">
-        <v>3.0</v>
-      </c>
-    </row>
-    <row r="36">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="C36" s="1" t="s">
         <v>10</v>
       </c>
       <c r="D36" s="10"/>
     </row>
-    <row r="37">
+    <row r="37" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="C37" s="1" t="s">
         <v>11</v>
       </c>
       <c r="D37" s="10"/>
     </row>
-    <row r="38">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A38" s="9">
-        <v>44673.0</v>
+        <v>44673</v>
       </c>
       <c r="C38" s="1">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="D38" s="11">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="F38" s="1">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="G38" s="1">
-        <v>2.0</v>
-      </c>
-    </row>
-    <row r="39">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="C39" s="1" t="s">
         <v>12</v>
       </c>
@@ -1017,24 +1039,24 @@
         <v>14</v>
       </c>
     </row>
-    <row r="40">
+    <row r="40" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D40" s="10"/>
     </row>
-    <row r="41">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A41" s="9">
-        <v>44674.0</v>
+        <v>44674</v>
       </c>
       <c r="C41" s="1">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="D41" s="11">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="G41" s="1">
-        <v>4.0</v>
-      </c>
-    </row>
-    <row r="42">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="C42" s="1" t="s">
         <v>15</v>
       </c>
@@ -1045,29 +1067,29 @@
         <v>17</v>
       </c>
     </row>
-    <row r="43">
+    <row r="43" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D43" s="11" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="44">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A44" s="9">
-        <v>44675.0</v>
+        <v>44675</v>
       </c>
       <c r="C44" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="D44" s="11">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="F44" s="1">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="G44" s="1">
-        <v>4.0</v>
-      </c>
-    </row>
-    <row r="45">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D45" s="11" t="s">
         <v>19</v>
       </c>
@@ -1076,33 +1098,33 @@
         <v>20</v>
       </c>
     </row>
-    <row r="46">
+    <row r="46" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D46" s="10"/>
       <c r="F46" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="47">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A47" s="9">
-        <v>44676.0</v>
+        <v>44676</v>
       </c>
       <c r="C47" s="1">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="D47" s="11">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="E47" s="1">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="F47" s="1">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="G47" s="1">
-        <v>4.0</v>
-      </c>
-    </row>
-    <row r="48">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="C48" s="1" t="s">
         <v>21</v>
       </c>
@@ -1117,30 +1139,30 @@
         <v>24</v>
       </c>
     </row>
-    <row r="49">
+    <row r="49" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="D49" s="10"/>
       <c r="E49" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="50">
+    <row r="50" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A50" s="9">
-        <v>44677.0</v>
+        <v>44677</v>
       </c>
       <c r="C50" s="1">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="D50" s="11">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="E50" s="1">
-        <v>7.0</v>
+        <v>7</v>
       </c>
       <c r="F50" s="1">
-        <v>2.0</v>
-      </c>
-    </row>
-    <row r="51">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="C51" s="1" t="s">
         <v>26</v>
       </c>
@@ -1154,30 +1176,30 @@
         <v>28</v>
       </c>
     </row>
-    <row r="52">
+    <row r="52" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="D52" s="10"/>
       <c r="E52" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="53">
+    <row r="53" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A53" s="9">
-        <v>44678.0</v>
+        <v>44678</v>
       </c>
       <c r="C53" s="1">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="D53" s="11">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="E53" s="1">
-        <v>6.0</v>
+        <v>6</v>
       </c>
       <c r="H53" s="1">
-        <v>4.0</v>
-      </c>
-    </row>
-    <row r="54">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="C54" s="1" t="s">
         <v>26</v>
       </c>
@@ -1188,7 +1210,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="55">
+    <row r="55" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="D55" s="11" t="s">
         <v>32</v>
       </c>
@@ -1196,24 +1218,24 @@
         <v>33</v>
       </c>
     </row>
-    <row r="56">
+    <row r="56" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A56" s="9">
-        <v>44679.0</v>
+        <v>44679</v>
       </c>
       <c r="C56" s="1">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="D56" s="11">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="E56" s="1">
-        <v>10.0</v>
+        <v>10</v>
       </c>
       <c r="H56" s="1">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="57">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="C57" s="1" t="s">
         <v>26</v>
       </c>
@@ -1224,30 +1246,30 @@
         <v>35</v>
       </c>
     </row>
-    <row r="58">
+    <row r="58" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="D58" s="10"/>
       <c r="E58" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="59">
+    <row r="59" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A59" s="9">
-        <v>44680.0</v>
+        <v>44680</v>
       </c>
       <c r="C59" s="1">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="D59" s="11">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="E59" s="1">
-        <v>7.0</v>
+        <v>7</v>
       </c>
       <c r="H59" s="12">
-        <v>2.0</v>
-      </c>
-    </row>
-    <row r="60">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="C60" s="1" t="s">
         <v>37</v>
       </c>
@@ -1258,49 +1280,49 @@
         <v>39</v>
       </c>
     </row>
-    <row r="61">
+    <row r="61" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="D61" s="10"/>
       <c r="E61" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="62">
+    <row r="62" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A62" s="9"/>
       <c r="D62" s="10"/>
     </row>
-    <row r="63">
+    <row r="63" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="B63" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C63" s="13">
-        <f t="shared" ref="C63:H63" si="2">SUM(C22:C60)</f>
+        <f t="shared" ref="C63:H63" si="1">SUM(C22:C60)</f>
         <v>24</v>
       </c>
       <c r="D63" s="10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>24</v>
       </c>
       <c r="E63" s="14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>37</v>
       </c>
       <c r="F63" s="14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>11</v>
       </c>
       <c r="G63" s="14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>30</v>
       </c>
       <c r="H63" s="14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>10</v>
       </c>
     </row>
-    <row r="64">
+    <row r="64" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="D64" s="10"/>
     </row>
-    <row r="65">
+    <row r="65" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="B65" s="3"/>
       <c r="D65" s="10"/>
       <c r="E65" s="14"/>
@@ -1308,24 +1330,24 @@
       <c r="G65" s="14"/>
       <c r="H65" s="14"/>
     </row>
-    <row r="66">
+    <row r="66" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A66" s="15">
-        <v>44683.0</v>
+        <v>44683</v>
       </c>
       <c r="C66" s="1">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="D66" s="1">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="E66" s="1">
-        <v>7.0</v>
+        <v>7</v>
       </c>
       <c r="H66" s="1">
-        <v>2.0</v>
-      </c>
-    </row>
-    <row r="67">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="C67" s="1" t="s">
         <v>41</v>
       </c>
@@ -1336,24 +1358,24 @@
         <v>43</v>
       </c>
     </row>
-    <row r="68">
+    <row r="68" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A68" s="15">
-        <v>44684.0</v>
+        <v>44684</v>
       </c>
       <c r="E68" s="1">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="F68" s="1">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="G68" s="1">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="H68" s="1">
-        <v>2.0</v>
-      </c>
-    </row>
-    <row r="69">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="E69" s="1" t="s">
         <v>44</v>
       </c>
@@ -1364,7 +1386,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="70">
+    <row r="70" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="F70" s="1" t="s">
         <v>46</v>
       </c>
@@ -1372,24 +1394,24 @@
         <v>46</v>
       </c>
     </row>
-    <row r="71">
+    <row r="71" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A71" s="15">
-        <v>44685.0</v>
+        <v>44685</v>
       </c>
       <c r="C71" s="1">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="D71" s="1">
-        <v>6.0</v>
+        <v>6</v>
       </c>
       <c r="F71" s="1">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="H71" s="1">
-        <v>5.0</v>
-      </c>
-    </row>
-    <row r="72">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="72" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="C72" s="1" t="s">
         <v>26</v>
       </c>
@@ -1400,26 +1422,26 @@
         <v>48</v>
       </c>
     </row>
-    <row r="73">
+    <row r="73" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="D73" s="16" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="74">
+    <row r="74" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A74" s="15">
-        <v>44686.0</v>
+        <v>44686</v>
       </c>
       <c r="C74" s="1">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="F74" s="1">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="H74" s="1">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="75">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="75" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="C75" s="1" t="s">
         <v>26</v>
       </c>
@@ -1427,18 +1449,18 @@
         <v>48</v>
       </c>
     </row>
-    <row r="77">
+    <row r="77" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A77" s="15">
-        <v>44687.0</v>
+        <v>44687</v>
       </c>
       <c r="C77" s="1">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="F77" s="1">
-        <v>4.0</v>
-      </c>
-    </row>
-    <row r="78">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="78" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="C78" s="1" t="s">
         <v>50</v>
       </c>
@@ -1446,52 +1468,65 @@
         <v>51</v>
       </c>
     </row>
-    <row r="79">
+    <row r="79" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="F79" s="1" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="80">
+    <row r="80" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A80" s="15">
-        <v>44688.0</v>
-      </c>
-    </row>
-    <row r="83">
+        <v>44688</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7" ht="13" x14ac:dyDescent="0.15">
       <c r="A83" s="15">
-        <v>44689.0</v>
-      </c>
-    </row>
-    <row r="86">
+        <v>44689</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7" ht="13" x14ac:dyDescent="0.15">
       <c r="A86" s="15">
-        <v>44690.0</v>
-      </c>
-    </row>
-    <row r="89">
+        <v>44690</v>
+      </c>
+      <c r="G86">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="G87" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="G88" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7" ht="13" x14ac:dyDescent="0.15">
       <c r="A89" s="15">
-        <v>44691.0</v>
-      </c>
-    </row>
-    <row r="92">
+        <v>44691</v>
+      </c>
+    </row>
+    <row r="92" spans="1:7" ht="13" x14ac:dyDescent="0.15">
       <c r="A92" s="15">
-        <v>44692.0</v>
-      </c>
-    </row>
-    <row r="95">
+        <v>44692</v>
+      </c>
+    </row>
+    <row r="95" spans="1:7" ht="13" x14ac:dyDescent="0.15">
       <c r="A95" s="15">
-        <v>44693.0</v>
-      </c>
-    </row>
-    <row r="98">
+        <v>44693</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" ht="13" x14ac:dyDescent="0.15">
       <c r="A98" s="15">
-        <v>44694.0</v>
-      </c>
-    </row>
-    <row r="101">
+        <v>44694</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" ht="13" x14ac:dyDescent="0.15">
       <c r="A101" s="15">
-        <v>44695.0</v>
-      </c>
-    </row>
-    <row r="104">
+        <v>44695</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" ht="13" x14ac:dyDescent="0.15">
       <c r="B104" s="1" t="s">
         <v>53</v>
       </c>
@@ -1500,26 +1535,27 @@
   <mergeCells count="1">
     <mergeCell ref="A3:B3"/>
   </mergeCells>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="B5:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col customWidth="1" min="4" max="4" width="47.38"/>
+    <col min="4" max="4" width="47.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="5" ht="45.0" customHeight="1">
+    <row r="5" spans="2:4" ht="45" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B5" s="17">
-        <v>44659.0</v>
+        <v>44659</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>54</v>
@@ -1529,6 +1565,6 @@
       </c>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>